<commit_message>
Addition of Seq Instrument Type to Normalization planning as well as index validation.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Normalization_planning_v3_13_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Normalization_planning_v3_13_0.xlsx
@@ -21,8 +21,31 @@
 </workbook>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>UFG</author>
+  </authors>
+  <commentList>
+    <comment ref="H3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">Used for index validation. If left empty, the validation will be skipped.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t xml:space="preserve">Sample and Library Normalization Planning Template</t>
   </si>
@@ -105,6 +128,9 @@
     <t xml:space="preserve">Pool Parent Container Coord</t>
   </si>
   <si>
+    <t xml:space="preserve">Seq Instrument Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Container Kind</t>
   </si>
   <si>
@@ -123,13 +149,25 @@
     <t xml:space="preserve">tube</t>
   </si>
   <si>
+    <t xml:space="preserve">Illumina MiSeq</t>
+  </si>
+  <si>
     <t xml:space="preserve">384-well plate</t>
   </si>
   <si>
     <t xml:space="preserve">Sample Biomek</t>
   </si>
   <si>
+    <t xml:space="preserve">Illumina NovaSeq 6000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample Janus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNBSEQ-G400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNBSEQ-T7</t>
   </si>
 </sst>
 </file>
@@ -140,7 +178,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -177,6 +215,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -255,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,6 +336,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -371,7 +426,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.86"/>
@@ -7244,13 +7299,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.91"/>
@@ -7259,6 +7314,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7296,6 +7352,9 @@
       <c r="G3" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="H3" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
@@ -7305,6 +7364,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7"/>
@@ -7314,6 +7374,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
@@ -7323,6 +7384,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
@@ -7332,6 +7394,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
@@ -7341,6 +7404,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
@@ -7350,6 +7414,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
@@ -7359,6 +7424,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
@@ -7368,6 +7434,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
@@ -7377,6 +7444,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
@@ -7386,6 +7454,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
@@ -7395,6 +7464,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
@@ -7404,6 +7474,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
@@ -7413,6 +7484,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
@@ -7422,6 +7494,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
@@ -7431,6 +7504,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
@@ -7440,6 +7514,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
@@ -7449,6 +7524,7 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7"/>
@@ -7458,6 +7534,7 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
@@ -7467,6 +7544,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
@@ -7476,6 +7554,7 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
@@ -7485,6 +7564,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
@@ -7494,6 +7574,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
@@ -7503,6 +7584,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7"/>
@@ -7512,6 +7594,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
@@ -7521,6 +7604,7 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7"/>
@@ -7530,6 +7614,7 @@
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
@@ -7539,6 +7624,7 @@
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7"/>
@@ -7548,6 +7634,7 @@
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7"/>
@@ -7557,6 +7644,7 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7"/>
@@ -7566,6 +7654,7 @@
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
@@ -7575,6 +7664,7 @@
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
@@ -7584,6 +7674,7 @@
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
@@ -7593,6 +7684,7 @@
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7"/>
@@ -7602,6 +7694,7 @@
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7"/>
@@ -7611,6 +7704,7 @@
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7"/>
@@ -7620,6 +7714,7 @@
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7"/>
@@ -7629,6 +7724,7 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7"/>
@@ -7638,6 +7734,7 @@
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="7"/>
@@ -7647,6 +7744,7 @@
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="7"/>
@@ -7656,6 +7754,7 @@
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="7"/>
@@ -7665,6 +7764,7 @@
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="7"/>
@@ -7674,6 +7774,7 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7"/>
@@ -7683,6 +7784,7 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7"/>
@@ -7692,6 +7794,7 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7"/>
@@ -7701,6 +7804,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="7"/>
@@ -7710,6 +7814,7 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7"/>
@@ -7719,6 +7824,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7"/>
@@ -7728,6 +7834,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7"/>
@@ -7737,6 +7844,7 @@
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7"/>
@@ -7746,6 +7854,7 @@
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7"/>
@@ -7755,6 +7864,7 @@
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7"/>
@@ -7764,6 +7874,7 @@
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7"/>
@@ -7773,6 +7884,7 @@
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7"/>
@@ -7782,6 +7894,7 @@
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7"/>
@@ -7791,6 +7904,7 @@
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7"/>
@@ -7800,6 +7914,7 @@
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7"/>
@@ -7809,6 +7924,7 @@
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7"/>
@@ -7818,6 +7934,7 @@
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7"/>
@@ -7827,6 +7944,7 @@
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7"/>
@@ -7836,6 +7954,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="7"/>
@@ -7845,6 +7964,7 @@
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7"/>
@@ -7854,6 +7974,7 @@
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7"/>
@@ -7863,6 +7984,7 @@
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7"/>
@@ -7872,6 +7994,7 @@
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7"/>
@@ -7881,6 +8004,7 @@
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7"/>
@@ -7890,6 +8014,7 @@
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7"/>
@@ -7899,6 +8024,7 @@
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7"/>
@@ -7908,6 +8034,7 @@
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7"/>
@@ -7917,6 +8044,7 @@
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7"/>
@@ -7926,6 +8054,7 @@
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7"/>
@@ -7935,6 +8064,7 @@
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7"/>
@@ -7944,6 +8074,7 @@
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7"/>
@@ -7953,6 +8084,7 @@
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7"/>
@@ -7962,6 +8094,7 @@
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="7"/>
@@ -7971,6 +8104,7 @@
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7"/>
@@ -7980,6 +8114,7 @@
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="7"/>
@@ -7989,6 +8124,7 @@
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="7"/>
@@ -7998,6 +8134,7 @@
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="7"/>
@@ -8007,6 +8144,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="7"/>
@@ -8016,6 +8154,7 @@
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7"/>
@@ -8025,6 +8164,7 @@
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7"/>
@@ -8034,6 +8174,7 @@
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="7"/>
@@ -8043,6 +8184,7 @@
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7"/>
@@ -8052,6 +8194,7 @@
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="7"/>
@@ -8061,6 +8204,7 @@
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7"/>
@@ -8070,6 +8214,7 @@
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7"/>
@@ -8079,6 +8224,7 @@
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7"/>
@@ -8088,6 +8234,7 @@
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="7"/>
@@ -8097,6 +8244,7 @@
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="7"/>
@@ -8106,6 +8254,7 @@
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="7"/>
@@ -8115,6 +8264,7 @@
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="7"/>
@@ -8124,6 +8274,7 @@
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
+      <c r="H95" s="7"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="7"/>
@@ -8133,6 +8284,7 @@
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="7"/>
@@ -8142,6 +8294,7 @@
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
       <c r="G97" s="7"/>
+      <c r="H97" s="7"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="7"/>
@@ -8171,9 +8324,13 @@
       <c r="G100" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4:E97" type="list">
       <formula1>Index!$C$2:$C$4</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H4:H97" type="list">
+      <formula1>Index!$D$2:$D$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -8184,6 +8341,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8192,59 +8350,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>30</v>
+      <c r="D3" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>33</v>
+      <c r="D4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>